<commit_message>
December 2015 - Polars implemeted
Polars implemented / debuged
Global parameters implemented / deleted Bundles
No TWA Gauge yet, still original boat with header
</commit_message>
<xml_diff>
--- a/Carpri25_Polars.xlsx
+++ b/Carpri25_Polars.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Google Drive\ProgramCode\Android\SailingRace\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Polars" sheetId="1" r:id="rId1"/>
     <sheet name="Plots" sheetId="2" r:id="rId2"/>
+    <sheet name="WT-VMG vs VMG-upwind" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Plots!$A$1:$I$60</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Wind</t>
   </si>
@@ -78,6 +78,27 @@
   <si>
     <t>True Wind Angle</t>
   </si>
+  <si>
+    <t> Windward Target Boat Speed</t>
+  </si>
+  <si>
+    <t>Downward Target Boat Speed</t>
+  </si>
+  <si>
+    <t>Downward TWA</t>
+  </si>
+  <si>
+    <t>calculated VMG-up</t>
+  </si>
+  <si>
+    <t>Upwind</t>
+  </si>
+  <si>
+    <t>Leeward Target VMG</t>
+  </si>
+  <si>
+    <t>Leeward Target Boat Speed</t>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +132,14 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -279,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,6 +356,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -351,12 +392,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -383,6 +455,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> Downward Target Boat Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -392,26 +489,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -424,11 +501,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plots!$L$2</c:f>
+              <c:f>Plots!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Windward Target VMG</c:v>
+                  <c:v>Downward Target Boat Speed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -489,7 +566,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="C00000"/>
                       </a:solidFill>
@@ -505,7 +582,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Plots!$K$3:$K$26</c:f>
+              <c:f>Plots!$T$3:$T$26</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="24"/>
@@ -567,7 +644,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>14</c:v>
@@ -586,81 +663,81 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Plots!$L$3:$L$26</c:f>
+              <c:f>Plots!$U$3:$U$26</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.9</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.2</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.2</c:v>
+                  <c:v>5.55</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.3</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.3</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.3</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.3</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,11 +752,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228542552"/>
-        <c:axId val="115271368"/>
+        <c:axId val="239699840"/>
+        <c:axId val="239701376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228542552"/>
+        <c:axId val="239699840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,12 +813,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115271368"/>
+        <c:crossAx val="239701376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115271368"/>
+        <c:axId val="239701376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +838,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -798,7 +875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228542552"/>
+        <c:crossAx val="239699840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -900,7 +977,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -913,7 +990,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>Windward True Wind Angle</a:t>
             </a:r>
           </a:p>
@@ -928,26 +1005,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1008,8 +1065,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.0332632085111427E-2"/>
-                  <c:y val="8.881443011112973E-2"/>
+                  <c:x val="-5.1993743480204378E-2"/>
+                  <c:y val="0.13865225863160546"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1103,7 +1160,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>14</c:v>
@@ -1211,11 +1268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="234438608"/>
-        <c:axId val="234439000"/>
+        <c:axId val="239543040"/>
+        <c:axId val="239544576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="234438608"/>
+        <c:axId val="239543040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,15 +1329,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234439000"/>
+        <c:crossAx val="239544576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="234439000"/>
+        <c:axId val="239544576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="20"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1335,7 +1392,1045 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234438608"/>
+        <c:crossAx val="239543040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Downward True</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Wind Angle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plots!$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Downward TWA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.3515938370299132E-2"/>
+                  <c:y val="0.41469108150337514"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plots!$W$3:$W$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plots!$X$3:$X$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="239594112"/>
+        <c:axId val="239600000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="239594112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="239600000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="239600000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="239594112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> Windward Target Boat Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plots!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Windward Target Boat Speed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.3515938370299132E-2"/>
+                  <c:y val="0.41469108150337514"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plots!$Q$3:$Q$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plots!$R$3:$R$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="240665728"/>
+        <c:axId val="240667264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="240665728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="240667264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="240667264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="240665728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2533,13 +3628,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>238124</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>376237</xdr:colOff>
+      <xdr:colOff>742949</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>219076</xdr:rowOff>
     </xdr:to>
@@ -2564,14 +3659,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>266701</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>249765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>376238</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>295274</xdr:rowOff>
+      <xdr:colOff>741382</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>189440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2585,6 +3680,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>243415</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>748240</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>240242</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2636,7 +3795,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2671,7 +3830,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2883,7 +4042,7 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M27"/>
+      <selection activeCell="H6" sqref="H6:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,10 +4063,10 @@
       <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2934,10 +4093,10 @@
       <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2964,10 +4123,10 @@
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3012,10 +4171,10 @@
       <c r="C6" s="8">
         <v>35</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="15">
         <v>0.6</v>
       </c>
@@ -3036,10 +4195,10 @@
         <v>47</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="19">
+      <c r="D7" s="23">
         <v>2.6</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="15">
         <v>0.9</v>
       </c>
@@ -3060,10 +4219,10 @@
         <v>47</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="19">
+      <c r="D8" s="23">
         <v>2.9</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="15">
         <v>1.2</v>
       </c>
@@ -3084,10 +4243,10 @@
         <v>47</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="19">
+      <c r="D9" s="23">
         <v>3.2</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="15">
         <v>1.5</v>
       </c>
@@ -3108,10 +4267,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="19">
+      <c r="D10" s="23">
         <v>3.5</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="15">
         <v>1.8</v>
       </c>
@@ -3134,10 +4293,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="19">
+      <c r="D11" s="23">
         <v>3.8</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="15">
         <v>2</v>
       </c>
@@ -3160,10 +4319,10 @@
         <v>47</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="19">
+      <c r="D12" s="23">
         <v>3.9</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="15">
         <v>2.2999999999999998</v>
       </c>
@@ -3186,10 +4345,10 @@
         <v>47</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="19">
+      <c r="D13" s="23">
         <v>4.2</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="15">
         <v>2.6</v>
       </c>
@@ -3214,10 +4373,10 @@
       <c r="C14" s="8">
         <v>34</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="23">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="15">
         <v>2.8</v>
       </c>
@@ -3242,10 +4401,10 @@
         <v>46</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="19">
+      <c r="D15" s="23">
         <v>4.5</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="15">
         <v>3</v>
       </c>
@@ -3270,10 +4429,10 @@
         <v>46</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="19">
+      <c r="D16" s="23">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="15">
         <v>3.2</v>
       </c>
@@ -3298,10 +4457,10 @@
         <v>46</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="19">
+      <c r="D17" s="23">
         <v>4.8</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="15">
         <v>3.3</v>
       </c>
@@ -3328,10 +4487,10 @@
       <c r="C18" s="8">
         <v>33</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="25">
         <v>5</v>
       </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="15">
         <v>3.5</v>
       </c>
@@ -3356,10 +4515,10 @@
         <v>45</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="19">
+      <c r="D19" s="23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E19" s="20"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="15">
         <v>3.7</v>
       </c>
@@ -3384,10 +4543,10 @@
         <v>45</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="19">
+      <c r="D20" s="23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E20" s="20"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="15">
         <v>3.8</v>
       </c>
@@ -3412,10 +4571,10 @@
         <v>45</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="19">
+      <c r="D21" s="23">
         <v>5.2</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="15">
         <v>3.9</v>
       </c>
@@ -3442,10 +4601,10 @@
       <c r="C22" s="8">
         <v>30</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="23">
         <v>5.2</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="15">
         <v>4</v>
       </c>
@@ -3470,10 +4629,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="19">
+      <c r="D23" s="23">
         <v>5.4</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="15">
         <v>4.0999999999999996</v>
       </c>
@@ -3498,10 +4657,10 @@
         <v>40</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="19">
+      <c r="D24" s="23">
         <v>5.5</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="15">
         <v>4.2</v>
       </c>
@@ -3526,15 +4685,15 @@
         <v>40</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="19">
+      <c r="D25" s="23">
         <v>5.5</v>
       </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="15">
         <v>4.2</v>
       </c>
       <c r="G25" s="15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H25" s="15">
         <v>5.4</v>
@@ -3550,10 +4709,10 @@
         <v>39</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="19">
+      <c r="D26" s="23">
         <v>5.6</v>
       </c>
-      <c r="E26" s="20"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="15">
         <v>4.3</v>
       </c>
@@ -3574,10 +4733,10 @@
         <v>38</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="19">
+      <c r="D27" s="23">
         <v>5.6</v>
       </c>
-      <c r="E27" s="20"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="15">
         <v>4.3</v>
       </c>
@@ -3628,20 +4787,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K1:O26"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="K1:Y39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="1" max="9" width="15.7109375" customWidth="1"/>
     <col min="11" max="12" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="11:15" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="11:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="11:25" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K2" s="16" t="s">
         <v>16</v>
       </c>
@@ -3654,12 +4819,31 @@
       <c r="O2" s="16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="19"/>
+      <c r="T2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K3" s="15">
         <v>2</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="22">
         <v>0.6</v>
       </c>
       <c r="N3" s="15">
@@ -3668,12 +4852,35 @@
       <c r="O3" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="15">
+        <v>2</v>
+      </c>
+      <c r="R3" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S3" s="19"/>
+      <c r="T3" s="15">
+        <v>2</v>
+      </c>
+      <c r="U3" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="W3" s="15">
+        <v>2</v>
+      </c>
+      <c r="X3" s="8">
+        <v>135</v>
+      </c>
+      <c r="Y3">
+        <f>180-X3</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K4" s="15">
         <v>2.5</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="22">
         <v>0.9</v>
       </c>
       <c r="M4" s="18"/>
@@ -3683,12 +4890,35 @@
       <c r="O4" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="R4" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="S4" s="19"/>
+      <c r="T4" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="U4" s="22">
+        <v>2.4</v>
+      </c>
+      <c r="W4" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="X4" s="8">
+        <v>135</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y26" si="0">180-X4</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="15">
         <v>3</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="22">
         <v>1.2</v>
       </c>
       <c r="N5" s="15">
@@ -3697,12 +4927,35 @@
       <c r="O5" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="15">
+        <v>3</v>
+      </c>
+      <c r="R5" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="S5" s="19"/>
+      <c r="T5" s="15">
+        <v>3</v>
+      </c>
+      <c r="U5" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="W5" s="15">
+        <v>3</v>
+      </c>
+      <c r="X5" s="8">
+        <v>138</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K6" s="15">
         <v>3.5</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="22">
         <v>1.5</v>
       </c>
       <c r="N6" s="15">
@@ -3711,12 +4964,35 @@
       <c r="O6" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q6" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="R6" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="S6" s="19"/>
+      <c r="T6" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="U6" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="W6" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="X6" s="8">
+        <v>138</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K7" s="15">
         <v>4</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="22">
         <v>1.8</v>
       </c>
       <c r="N7" s="15">
@@ -3725,12 +5001,35 @@
       <c r="O7" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="15">
+        <v>4</v>
+      </c>
+      <c r="R7" s="21">
+        <v>3.5</v>
+      </c>
+      <c r="S7" s="19"/>
+      <c r="T7" s="15">
+        <v>4</v>
+      </c>
+      <c r="U7" s="22">
+        <v>3</v>
+      </c>
+      <c r="W7" s="15">
+        <v>4</v>
+      </c>
+      <c r="X7" s="8">
+        <v>138</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="15">
         <v>4.5</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="22">
         <v>2</v>
       </c>
       <c r="N8" s="15">
@@ -3739,12 +5038,35 @@
       <c r="O8" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="R8" s="21">
+        <v>3.8</v>
+      </c>
+      <c r="S8" s="19"/>
+      <c r="T8" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="U8" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="W8" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="X8" s="8">
+        <v>142</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K9" s="15">
         <v>5</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="22">
         <v>2.2999999999999998</v>
       </c>
       <c r="N9" s="15">
@@ -3753,12 +5075,35 @@
       <c r="O9" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q9" s="15">
+        <v>5</v>
+      </c>
+      <c r="R9" s="21">
+        <v>4</v>
+      </c>
+      <c r="S9" s="19"/>
+      <c r="T9" s="15">
+        <v>5</v>
+      </c>
+      <c r="U9" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="W9" s="15">
+        <v>5</v>
+      </c>
+      <c r="X9" s="8">
+        <v>142</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K10" s="15">
         <v>5.5</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="22">
         <v>2.6</v>
       </c>
       <c r="N10" s="15">
@@ -3767,12 +5112,35 @@
       <c r="O10" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="R10" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="S10" s="19"/>
+      <c r="T10" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="U10" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="W10" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="X10" s="8">
+        <v>142</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K11" s="15">
         <v>6</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="22">
         <v>2.8</v>
       </c>
       <c r="N11" s="15">
@@ -3781,12 +5149,35 @@
       <c r="O11" s="8">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="15">
+        <v>6</v>
+      </c>
+      <c r="R11" s="21">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S11" s="19"/>
+      <c r="T11" s="15">
+        <v>6</v>
+      </c>
+      <c r="U11" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="W11" s="15">
+        <v>6</v>
+      </c>
+      <c r="X11" s="8">
+        <v>146</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K12" s="15">
         <v>6.5</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="22">
         <v>3</v>
       </c>
       <c r="N12" s="15">
@@ -3795,12 +5186,35 @@
       <c r="O12" s="8">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="R12" s="21">
+        <v>4.5</v>
+      </c>
+      <c r="S12" s="19"/>
+      <c r="T12" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="U12" s="22">
+        <v>3.9</v>
+      </c>
+      <c r="W12" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="X12" s="8">
+        <v>150</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K13" s="15">
         <v>7</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="22">
         <v>3.2</v>
       </c>
       <c r="N13" s="15">
@@ -3809,12 +5223,35 @@
       <c r="O13" s="8">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="15">
+        <v>7</v>
+      </c>
+      <c r="R13" s="21">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="S13" s="19"/>
+      <c r="T13" s="15">
+        <v>7</v>
+      </c>
+      <c r="U13" s="22">
+        <v>4</v>
+      </c>
+      <c r="W13" s="15">
+        <v>7</v>
+      </c>
+      <c r="X13" s="8">
+        <v>155</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K14" s="15">
         <v>7.5</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="22">
         <v>3.3</v>
       </c>
       <c r="N14" s="15">
@@ -3823,12 +5260,35 @@
       <c r="O14" s="8">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="R14" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="S14" s="20"/>
+      <c r="T14" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="U14" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W14" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="X14" s="8">
+        <v>159</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="15">
         <v>8</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="22">
         <v>3.5</v>
       </c>
       <c r="N15" s="15">
@@ -3837,12 +5297,35 @@
       <c r="O15" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q15" s="15">
+        <v>8</v>
+      </c>
+      <c r="R15" s="21">
+        <v>5</v>
+      </c>
+      <c r="S15" s="19"/>
+      <c r="T15" s="15">
+        <v>8</v>
+      </c>
+      <c r="U15" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="W15" s="15">
+        <v>8</v>
+      </c>
+      <c r="X15" s="8">
+        <v>162</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K16" s="15">
         <v>8.5</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="22">
         <v>3.7</v>
       </c>
       <c r="N16" s="15">
@@ -3851,12 +5334,35 @@
       <c r="O16" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="R16" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S16" s="19"/>
+      <c r="T16" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="U16" s="22">
+        <v>4.3</v>
+      </c>
+      <c r="W16" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="X16" s="8">
+        <v>165</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K17" s="15">
         <v>9</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="22">
         <v>3.8</v>
       </c>
       <c r="N17" s="15">
@@ -3865,12 +5371,35 @@
       <c r="O17" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="15">
+        <v>9</v>
+      </c>
+      <c r="R17" s="21">
+        <v>5.15</v>
+      </c>
+      <c r="S17" s="19"/>
+      <c r="T17" s="15">
+        <v>9</v>
+      </c>
+      <c r="U17" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="W17" s="15">
+        <v>9</v>
+      </c>
+      <c r="X17" s="8">
+        <v>167</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K18" s="15">
         <v>9.5</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="22">
         <v>3.9</v>
       </c>
       <c r="N18" s="15">
@@ -3879,12 +5408,35 @@
       <c r="O18" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q18" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="R18" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="S18" s="19"/>
+      <c r="T18" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="U18" s="22">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="W18" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="X18" s="8">
+        <v>170</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K19" s="15">
         <v>10</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L19" s="22">
         <v>4</v>
       </c>
       <c r="N19" s="15">
@@ -3893,12 +5445,35 @@
       <c r="O19" s="8">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="15">
+        <v>10</v>
+      </c>
+      <c r="R19" s="21">
+        <v>5.3</v>
+      </c>
+      <c r="S19" s="19"/>
+      <c r="T19" s="15">
+        <v>10</v>
+      </c>
+      <c r="U19" s="22">
+        <v>4.8</v>
+      </c>
+      <c r="W19" s="15">
+        <v>10</v>
+      </c>
+      <c r="X19" s="8">
+        <v>170</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K20" s="15">
         <v>11</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="22">
         <v>4.0999999999999996</v>
       </c>
       <c r="N20" s="15">
@@ -3907,12 +5482,35 @@
       <c r="O20" s="8">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="15">
+        <v>11</v>
+      </c>
+      <c r="R20" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="S20" s="19"/>
+      <c r="T20" s="15">
+        <v>11</v>
+      </c>
+      <c r="U20" s="22">
+        <v>5</v>
+      </c>
+      <c r="W20" s="15">
+        <v>11</v>
+      </c>
+      <c r="X20" s="8">
+        <v>170</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K21" s="15">
         <v>12</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="22">
         <v>4.2</v>
       </c>
       <c r="N21" s="15">
@@ -3921,26 +5519,72 @@
       <c r="O21" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q21" s="15">
+        <v>12</v>
+      </c>
+      <c r="R21" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="S21" s="19"/>
+      <c r="T21" s="15">
+        <v>12</v>
+      </c>
+      <c r="U21" s="22">
+        <v>5.4</v>
+      </c>
+      <c r="W21" s="15">
+        <v>12</v>
+      </c>
+      <c r="X21" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K22" s="15">
-        <v>12</v>
-      </c>
-      <c r="L22" s="15">
+        <v>13</v>
+      </c>
+      <c r="L22" s="22">
         <v>4.2</v>
       </c>
       <c r="N22" s="15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O22" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="15">
+        <v>13</v>
+      </c>
+      <c r="R22" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="S22" s="19"/>
+      <c r="T22" s="15">
+        <v>13</v>
+      </c>
+      <c r="U22" s="22">
+        <v>5.55</v>
+      </c>
+      <c r="W22" s="15">
+        <v>13</v>
+      </c>
+      <c r="X22" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K23" s="15">
         <v>14</v>
       </c>
-      <c r="L23" s="15">
+      <c r="L23" s="22">
         <v>4.3</v>
       </c>
       <c r="N23" s="15">
@@ -3949,12 +5593,35 @@
       <c r="O23" s="8">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="15">
+        <v>14</v>
+      </c>
+      <c r="R23" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="S23" s="19"/>
+      <c r="T23" s="15">
+        <v>14</v>
+      </c>
+      <c r="U23" s="22">
+        <v>5.9</v>
+      </c>
+      <c r="W23" s="15">
+        <v>14</v>
+      </c>
+      <c r="X23" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K24" s="15">
         <v>15</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="22">
         <v>4.3</v>
       </c>
       <c r="N24" s="15">
@@ -3963,12 +5630,34 @@
       <c r="O24" s="8">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="15">
+        <v>15</v>
+      </c>
+      <c r="R24" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="T24" s="15">
+        <v>15</v>
+      </c>
+      <c r="U24" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="W24" s="15">
+        <v>15</v>
+      </c>
+      <c r="X24" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K25" s="15">
         <v>16</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="22">
         <v>4.3</v>
       </c>
       <c r="N25" s="15">
@@ -3977,12 +5666,34 @@
       <c r="O25" s="8">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="11:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q25" s="15">
+        <v>16</v>
+      </c>
+      <c r="R25" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="T25" s="15">
+        <v>16</v>
+      </c>
+      <c r="U25" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="W25" s="15">
+        <v>16</v>
+      </c>
+      <c r="X25" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="11:25" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K26" s="15">
         <v>17</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="22">
         <v>4.3</v>
       </c>
       <c r="N26" s="15">
@@ -3991,10 +5702,883 @@
       <c r="O26" s="8">
         <v>38</v>
       </c>
-    </row>
+      <c r="Q26" s="15">
+        <v>17</v>
+      </c>
+      <c r="R26" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="T26" s="15">
+        <v>17</v>
+      </c>
+      <c r="U26" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="W26" s="15">
+        <v>17</v>
+      </c>
+      <c r="X26" s="8">
+        <v>173</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="11:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="59" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;8Volker Petersen&amp;R&amp;8&amp;F+&amp;A</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" customWidth="1"/>
+    <col min="15" max="20" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="I2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>47</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="G5" s="22">
+        <f>C5*COS(RADIANS(B5))</f>
+        <v>1.5685962281437464</v>
+      </c>
+      <c r="I5" s="15">
+        <v>2</v>
+      </c>
+      <c r="J5" s="8">
+        <v>135</v>
+      </c>
+      <c r="K5" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="M5" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="O5" s="22">
+        <f>K5*COS(RADIANS(180-J5))</f>
+        <v>1.48492424049175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>47</v>
+      </c>
+      <c r="C6" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="22">
+        <f t="shared" ref="G6:G26" si="0">C6*COS(RADIANS(B6))</f>
+        <v>1.7731957361624962</v>
+      </c>
+      <c r="I6" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>135</v>
+      </c>
+      <c r="K6" s="22">
+        <v>2.4</v>
+      </c>
+      <c r="M6" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="O6" s="22">
+        <f t="shared" ref="O6:O26" si="1">K6*COS(RADIANS(180-J6))</f>
+        <v>1.697056274847714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>47</v>
+      </c>
+      <c r="C7" s="22">
+        <v>2.9</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" si="0"/>
+        <v>1.9777952441812454</v>
+      </c>
+      <c r="I7" s="15">
+        <v>3</v>
+      </c>
+      <c r="J7" s="8">
+        <v>138</v>
+      </c>
+      <c r="K7" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="M7" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="O7" s="22">
+        <f t="shared" si="1"/>
+        <v>1.932176546241225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>47</v>
+      </c>
+      <c r="C8" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="22">
+        <f t="shared" si="0"/>
+        <v>2.1823947521999951</v>
+      </c>
+      <c r="I8" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>138</v>
+      </c>
+      <c r="K8" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="M8" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="O8" s="22">
+        <f t="shared" si="1"/>
+        <v>2.0808055113367039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>47</v>
+      </c>
+      <c r="C9" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="G9" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3869942602187448</v>
+      </c>
+      <c r="I9" s="15">
+        <v>4</v>
+      </c>
+      <c r="J9" s="8">
+        <v>138</v>
+      </c>
+      <c r="K9" s="22">
+        <v>3</v>
+      </c>
+      <c r="M9" s="15">
+        <v>3</v>
+      </c>
+      <c r="O9" s="22">
+        <f t="shared" si="1"/>
+        <v>2.229434476432183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>47</v>
+      </c>
+      <c r="C10" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="E10" s="15">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5915937682374941</v>
+      </c>
+      <c r="I10" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="J10" s="8">
+        <v>142</v>
+      </c>
+      <c r="K10" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="M10" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="O10" s="22">
+        <f t="shared" si="1"/>
+        <v>2.5216344115415104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>47</v>
+      </c>
+      <c r="C11" s="22">
+        <v>4</v>
+      </c>
+      <c r="E11" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7279934402499939</v>
+      </c>
+      <c r="I11" s="15">
+        <v>5</v>
+      </c>
+      <c r="J11" s="8">
+        <v>142</v>
+      </c>
+      <c r="K11" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="M11" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="O11" s="22">
+        <f t="shared" si="1"/>
+        <v>2.7580376376235267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>47</v>
+      </c>
+      <c r="C12" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="E12" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="0"/>
+        <v>2.8643931122624937</v>
+      </c>
+      <c r="I12" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="J12" s="8">
+        <v>142</v>
+      </c>
+      <c r="K12" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="M12" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="1"/>
+        <v>2.9156397883448713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8">
+        <v>46</v>
+      </c>
+      <c r="C13" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E13" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="G13" s="22">
+        <f t="shared" si="0"/>
+        <v>3.0564968300195883</v>
+      </c>
+      <c r="I13" s="15">
+        <v>6</v>
+      </c>
+      <c r="J13" s="8">
+        <v>146</v>
+      </c>
+      <c r="K13" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="M13" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="O13" s="22">
+        <f t="shared" si="1"/>
+        <v>3.150342775709158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="B14" s="8">
+        <v>46</v>
+      </c>
+      <c r="C14" s="22">
+        <v>4.5</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="0"/>
+        <v>3.1259626670654876</v>
+      </c>
+      <c r="I14" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>150</v>
+      </c>
+      <c r="K14" s="22">
+        <v>3.9</v>
+      </c>
+      <c r="M14" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="O14" s="22">
+        <f t="shared" si="1"/>
+        <v>3.377499074759311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <v>46</v>
+      </c>
+      <c r="C15" s="22">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E15" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="0"/>
+        <v>3.2301614226343376</v>
+      </c>
+      <c r="I15" s="15">
+        <v>7</v>
+      </c>
+      <c r="J15" s="8">
+        <v>155</v>
+      </c>
+      <c r="K15" s="22">
+        <v>4</v>
+      </c>
+      <c r="M15" s="15">
+        <v>4</v>
+      </c>
+      <c r="O15" s="22">
+        <f t="shared" si="1"/>
+        <v>3.6252311481465997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>46</v>
+      </c>
+      <c r="C16" s="22">
+        <v>4.8</v>
+      </c>
+      <c r="E16" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="0"/>
+        <v>3.3343601782031866</v>
+      </c>
+      <c r="I16" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>159</v>
+      </c>
+      <c r="K16" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M16" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O16" s="22">
+        <f t="shared" si="1"/>
+        <v>3.827679748638527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
+        <v>8</v>
+      </c>
+      <c r="B17" s="8">
+        <v>45</v>
+      </c>
+      <c r="C17" s="22">
+        <v>5</v>
+      </c>
+      <c r="E17" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="G17" s="22">
+        <f t="shared" si="0"/>
+        <v>3.5355339059327378</v>
+      </c>
+      <c r="I17" s="15">
+        <v>8</v>
+      </c>
+      <c r="J17" s="8">
+        <v>162</v>
+      </c>
+      <c r="K17" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="M17" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="1"/>
+        <v>3.994437368439645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="B18" s="8">
+        <v>45</v>
+      </c>
+      <c r="C18" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E18" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6062445840513924</v>
+      </c>
+      <c r="I18" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="J18" s="8">
+        <v>165</v>
+      </c>
+      <c r="K18" s="22">
+        <v>4.3</v>
+      </c>
+      <c r="M18" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="O18" s="22">
+        <f t="shared" si="1"/>
+        <v>4.1534810530429933</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>9</v>
+      </c>
+      <c r="B19" s="8">
+        <v>45</v>
+      </c>
+      <c r="C19" s="22">
+        <v>5.15</v>
+      </c>
+      <c r="E19" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6415999231107201</v>
+      </c>
+      <c r="I19" s="15">
+        <v>9</v>
+      </c>
+      <c r="J19" s="8">
+        <v>167</v>
+      </c>
+      <c r="K19" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M19" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="O19" s="22">
+        <f t="shared" si="1"/>
+        <v>4.2872282850550354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>45</v>
+      </c>
+      <c r="C20" s="22">
+        <v>5.2</v>
+      </c>
+      <c r="E20" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6769552621700474</v>
+      </c>
+      <c r="I20" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="J20" s="8">
+        <v>170</v>
+      </c>
+      <c r="K20" s="22">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M20" s="15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O20" s="22">
+        <f t="shared" si="1"/>
+        <v>4.5301156638561562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>10</v>
+      </c>
+      <c r="B21" s="8">
+        <v>42</v>
+      </c>
+      <c r="C21" s="22">
+        <v>5.3</v>
+      </c>
+      <c r="E21" s="15">
+        <v>4</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>3.9386675750301894</v>
+      </c>
+      <c r="I21" s="15">
+        <v>10</v>
+      </c>
+      <c r="J21" s="8">
+        <v>170</v>
+      </c>
+      <c r="K21" s="22">
+        <v>4.8</v>
+      </c>
+      <c r="M21" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="O21" s="22">
+        <f t="shared" si="1"/>
+        <v>4.727077214458598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8">
+        <v>42</v>
+      </c>
+      <c r="C22" s="22">
+        <v>5.4</v>
+      </c>
+      <c r="E22" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" si="0"/>
+        <v>4.0129820575779291</v>
+      </c>
+      <c r="I22" s="15">
+        <v>11</v>
+      </c>
+      <c r="J22" s="8">
+        <v>170</v>
+      </c>
+      <c r="K22" s="22">
+        <v>5</v>
+      </c>
+      <c r="M22" s="15">
+        <v>5</v>
+      </c>
+      <c r="O22" s="22">
+        <f t="shared" si="1"/>
+        <v>4.9240387650610398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>12</v>
+      </c>
+      <c r="B23" s="8">
+        <v>40</v>
+      </c>
+      <c r="C23" s="22">
+        <v>5.5</v>
+      </c>
+      <c r="E23" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="0"/>
+        <v>4.2132444371543789</v>
+      </c>
+      <c r="I23" s="15">
+        <v>12</v>
+      </c>
+      <c r="J23" s="8">
+        <v>173</v>
+      </c>
+      <c r="K23" s="22">
+        <v>5.4</v>
+      </c>
+      <c r="M23" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="O23" s="22">
+        <f t="shared" si="1"/>
+        <v>5.359749218863139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
+        <v>13</v>
+      </c>
+      <c r="B24" s="8">
+        <v>40</v>
+      </c>
+      <c r="C24" s="22">
+        <v>5.5</v>
+      </c>
+      <c r="E24" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>4.2132444371543789</v>
+      </c>
+      <c r="I24" s="15">
+        <v>13</v>
+      </c>
+      <c r="J24" s="8">
+        <v>173</v>
+      </c>
+      <c r="K24" s="22">
+        <v>5.55</v>
+      </c>
+      <c r="M24" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="O24" s="22">
+        <f t="shared" si="1"/>
+        <v>5.508631141609337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
+        <v>14</v>
+      </c>
+      <c r="B25" s="8">
+        <v>39</v>
+      </c>
+      <c r="C25" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="E25" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="0"/>
+        <v>4.3520173841590371</v>
+      </c>
+      <c r="I25" s="15">
+        <v>14</v>
+      </c>
+      <c r="J25" s="8">
+        <v>173</v>
+      </c>
+      <c r="K25" s="22">
+        <v>5.9</v>
+      </c>
+      <c r="M25" s="15">
+        <v>5.9</v>
+      </c>
+      <c r="O25" s="22">
+        <f t="shared" si="1"/>
+        <v>5.8560222946838003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
+        <v>15</v>
+      </c>
+      <c r="B26" s="8">
+        <v>38</v>
+      </c>
+      <c r="C26" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="E26" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="0"/>
+        <v>4.4128602201976426</v>
+      </c>
+      <c r="I26" s="15">
+        <v>15</v>
+      </c>
+      <c r="J26" s="8">
+        <v>173</v>
+      </c>
+      <c r="K26" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="M26" s="15">
+        <v>6.1</v>
+      </c>
+      <c r="O26" s="22">
+        <f t="shared" si="1"/>
+        <v>6.0545315250120639</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="I2:O2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>